<commit_message>
Xuất báo cáo excel (Tạm thời ổn)
</commit_message>
<xml_diff>
--- a/HBM_HR_Admin_Angular2/hbm_hr_admin_angular2.client/public/assets/template.xlsx
+++ b/HBM_HR_Admin_Angular2/hbm_hr_admin_angular2.client/public/assets/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\admin\hbm_hr_admin\HBM_HR_Admin_Angular2\hbm_hr_admin_angular2.client\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC83ED6-3F85-46E1-B516-709A403CB270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C378BD-4C74-480E-A2DE-04FF47F368A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BD0D9CD-2DA5-4F2C-870E-379884894E3C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Chủ đề</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>{{/questions}}</t>
+  </si>
+  <si>
+    <t>{{totalParticip}}</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,8 +585,8 @@
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="9">
-        <v>1</v>
+      <c r="B5" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
xuất báo cáo ra file excel tạm ổn
</commit_message>
<xml_diff>
--- a/HBM_HR_Admin_Angular2/hbm_hr_admin_angular2.client/public/assets/template.xlsx
+++ b/HBM_HR_Admin_Angular2/hbm_hr_admin_angular2.client/public/assets/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\admin\hbm_hr_admin\HBM_HR_Admin_Angular2\hbm_hr_admin_angular2.client\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C378BD-4C74-480E-A2DE-04FF47F368A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{928AABA1-3808-4984-BF32-18AA7DB58043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2BD0D9CD-2DA5-4F2C-870E-379884894E3C}"/>
   </bookViews>
@@ -66,31 +66,31 @@
     <t>{{/options}}</t>
   </si>
   <si>
+    <t>{{title}}</t>
+  </si>
+  <si>
+    <t>{{description}}</t>
+  </si>
+  <si>
+    <t>{{startDate}}</t>
+  </si>
+  <si>
+    <t>{{endDate}}</t>
+  </si>
+  <si>
+    <t>{{/questions}}</t>
+  </si>
+  <si>
+    <t>{{totalParticip}}</t>
+  </si>
+  <si>
+    <t>{{questionContent}}</t>
+  </si>
+  <si>
+    <t>{{optionContent}}</t>
+  </si>
+  <si>
     <t>{{selectedCount}}</t>
-  </si>
-  <si>
-    <t>{{title}}</t>
-  </si>
-  <si>
-    <t>{{description}}</t>
-  </si>
-  <si>
-    <t>{{startDate}}</t>
-  </si>
-  <si>
-    <t>{{endDate}}</t>
-  </si>
-  <si>
-    <t>{{questionContent}}</t>
-  </si>
-  <si>
-    <t>{{optionContent}}</t>
-  </si>
-  <si>
-    <t>{{/questions}}</t>
-  </si>
-  <si>
-    <t>{{totalParticip}}</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,7 +553,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -570,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -578,7 +578,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,7 +599,7 @@
     </row>
     <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -607,10 +607,10 @@
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -624,7 +624,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>